<commit_message>
Actualizado Kanvan y registro, reunión 03/12/2024
</commit_message>
<xml_diff>
--- a/kanban_sprint2.xlsx
+++ b/kanban_sprint2.xlsx
@@ -78,7 +78,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -121,6 +121,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -203,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,11 +246,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,8 +521,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,20 +585,20 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="9"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
@@ -596,7 +606,7 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
@@ -604,7 +614,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
@@ -612,7 +622,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="9"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Corregido error en Kanban y registro, reunión 03/12/2024
</commit_message>
<xml_diff>
--- a/kanban_sprint2.xlsx
+++ b/kanban_sprint2.xlsx
@@ -209,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,6 +247,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -521,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -589,16 +593,16 @@
       <c r="C6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="8" t="s">
@@ -606,7 +610,7 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="8" t="s">
@@ -614,7 +618,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
@@ -622,7 +626,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Actualizado Kanban y registro, reunión 07/12/2024
</commit_message>
<xml_diff>
--- a/kanban_sprint2.xlsx
+++ b/kanban_sprint2.xlsx
@@ -246,11 +246,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,7 +526,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -590,10 +590,10 @@
     </row>
     <row r="6" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10"/>
       <c r="E6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Actualizado Kanban y registro, reunión 08/12/2024
</commit_message>
<xml_diff>
--- a/kanban_sprint2.xlsx
+++ b/kanban_sprint2.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Tarea 1:  Diagrama Entidad Relación de la BBDD a realizar y paso a tabla del diagrama. Asignada a Carlos Megías</t>
   </si>
   <si>
-    <t xml:space="preserve">Tarea2:   Creación de un XML Schema para representar los datos de una de las compañias (registro de la tabla de la BBDD). Asignada a Erik Flaquer</t>
+    <t xml:space="preserve">Tarea 2:   Creación de un XML Schema para representar los datos de una de las compañias (registro de la tabla de la BBDD). Asignada a Erik Flaquer</t>
   </si>
   <si>
     <t xml:space="preserve">Tarea 3:  Diagrama de clases UML del proyecto (con la Clase Empresa y con la Clase IndiceEmpresas). Asignada Aníbal Zambrana</t>
@@ -78,7 +78,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -135,6 +135,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -209,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,6 +256,30 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,20 +288,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -525,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -591,42 +609,42 @@
     <row r="6" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
       <c r="E7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="11"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Actualizado Kanban y registro, reunión 09/12/2024
</commit_message>
<xml_diff>
--- a/kanban_sprint2.xlsx
+++ b/kanban_sprint2.xlsx
@@ -78,7 +78,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -126,12 +126,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -139,7 +133,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -215,7 +209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -260,11 +254,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,7 +266,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,16 +274,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -543,8 +533,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -625,14 +615,14 @@
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="8"/>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="6"/>
@@ -641,10 +631,10 @@
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Actualizado Kanban y registro, reunión 10/12/2024
</commit_message>
<xml_diff>
--- a/kanban_sprint2.xlsx
+++ b/kanban_sprint2.xlsx
@@ -78,7 +78,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -128,6 +128,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -209,7 +215,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,15 +276,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -533,8 +535,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -607,32 +609,32 @@
     <row r="7" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="12"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="8"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="11" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>